<commit_message>
feat: add lead rotation script and base template with login-protected Excel reload
</commit_message>
<xml_diff>
--- a/data_prueba.xlsx
+++ b/data_prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbeno\CascadeProjects\tuotempo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE9AED6-6CD8-455F-8627-F41CFD1553AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3C6A43-D473-445B-88D9-99C4B6E03A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -314,9 +314,9 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,6 +332,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -369,22 +377,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -689,8 +700,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AD1501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AB5" sqref="AB5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1081,7 +1092,7 @@
       <c r="AA5" t="s">
         <v>66</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AB5" s="5" t="s">
         <v>67</v>
       </c>
       <c r="AC5" t="s">
@@ -5864,6 +5875,9 @@
       <c r="P1501" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="AB5" r:id="rId1" xr:uid="{07C83C71-6E22-4F9C-A73D-FC58927887A3}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>